<commit_message>
Ultra-Premium Presentation Overhaul: Slide split, Dashboard optimization, and Screen-fit refinements
</commit_message>
<xml_diff>
--- a/1st Visit/1st visit.xlsx
+++ b/1st Visit/1st visit.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aqeel\Desktop\shorkipresentation\1st Visit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCE5E1A-C25D-4F3D-93D4-2D12F2257D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>S NO</t>
   </si>
@@ -137,14 +132,14 @@
     <t>Madian ( fungicides )</t>
   </si>
   <si>
-    <t>INVENTORY SHEET FOR SHORKI WHAREHOUSE Ist Visit</t>
+    <t xml:space="preserve">FIRST VISIT INVENTORY SHEET OF SHORKI STORE </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,7 +149,29 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -192,25 +209,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,404 +595,476 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="6.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="84" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.77734375" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="6" t="s">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D4" s="2" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D5" s="5">
+      <c r="E5" s="8"/>
+      <c r="F5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5">
+      <c r="D6" s="12">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D6" s="5">
+      <c r="E6" s="13"/>
+      <c r="F6" s="14">
+        <v>17</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10">
+        <v>4</v>
+      </c>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="C7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="5">
+      <c r="D7" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D7" s="5">
+      <c r="E7" s="13"/>
+      <c r="F7" s="14">
+        <v>18</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="10">
+        <v>6</v>
+      </c>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="C8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="5">
+      <c r="D8" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D8" s="5">
+      <c r="E8" s="13"/>
+      <c r="F8" s="14">
+        <v>19</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="10">
+        <v>3</v>
+      </c>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="10">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="C9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="5">
+      <c r="D9" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D9" s="5">
+      <c r="E9" s="13"/>
+      <c r="F9" s="14">
+        <v>20</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="10">
+        <v>4</v>
+      </c>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="C10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="5">
+      <c r="D10" s="12">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D10" s="5">
+      <c r="E10" s="13"/>
+      <c r="F10" s="14">
+        <v>21</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="10">
+        <v>13</v>
+      </c>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="10">
         <v>6</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="C11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="5">
+      <c r="D11" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D11" s="5">
+      <c r="E11" s="13"/>
+      <c r="F11" s="14">
+        <v>22</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="10">
+        <v>17</v>
+      </c>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="10">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="C12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="5">
+      <c r="D12" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D12" s="5">
+      <c r="E12" s="13"/>
+      <c r="F12" s="14">
+        <v>23</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="10">
         <v>8</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="C13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="5">
+      <c r="D13" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D13" s="5">
+      <c r="E13" s="13"/>
+      <c r="F13" s="14">
+        <v>24</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="10">
+        <v>20</v>
+      </c>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="10">
         <v>9</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="C14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="5">
+      <c r="D14" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D14" s="5">
+      <c r="E14" s="13"/>
+      <c r="F14" s="14">
+        <v>25</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="10">
+        <v>20</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="10">
         <v>10</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="C15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="5">
+      <c r="D15" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D15" s="5">
+      <c r="E15" s="13"/>
+      <c r="F15" s="14">
+        <v>26</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="10">
+        <v>400</v>
+      </c>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="10">
         <v>11</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="C16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="5">
+      <c r="D16" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D16" s="5">
+      <c r="E16" s="13"/>
+      <c r="F16" s="14">
+        <v>27</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="10">
         <v>12</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="10">
+        <v>12</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="5">
+      <c r="D17" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D17" s="5">
+      <c r="E17" s="13"/>
+      <c r="F17" s="14">
+        <v>28</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="10">
+        <v>2</v>
+      </c>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="10">
         <v>13</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="C18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="5">
+      <c r="D18" s="12">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D18" s="5">
+      <c r="E18" s="13"/>
+      <c r="F18" s="14">
+        <v>29</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="10">
+        <v>6</v>
+      </c>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="10">
         <v>14</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="C19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="5">
+      <c r="D19" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D19" s="5">
+      <c r="E19" s="13"/>
+      <c r="F19" s="14">
+        <v>30</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="10">
+        <v>6</v>
+      </c>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="10">
         <v>15</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="C20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="5">
+      <c r="D20" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D20" s="5">
+      <c r="E20" s="13"/>
+      <c r="F20" s="14">
+        <v>31</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="10">
+        <v>2</v>
+      </c>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="10">
         <v>16</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="C21" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="5">
+      <c r="D21" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D21" s="5">
-        <v>17</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D22" s="5">
-        <v>18</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D23" s="5">
-        <v>19</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D24" s="5">
+      <c r="E21" s="16"/>
+      <c r="F21" s="14">
+        <v>32</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D25" s="5">
-        <v>21</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D26" s="5">
-        <v>22</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="5">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D27" s="5">
-        <v>23</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D28" s="5">
-        <v>24</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D29" s="5">
-        <v>25</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D30" s="5">
-        <v>26</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D31" s="5">
-        <v>27</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D32" s="5">
-        <v>28</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D33" s="5">
-        <v>29</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D34" s="5">
-        <v>30</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D35" s="5">
-        <v>31</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F35" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D36" s="5">
-        <v>32</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="5">
+      <c r="H21" s="10">
         <v>66</v>
       </c>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B3:H3"/>
   </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="110" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>